<commit_message>
Add function to fix German encoding issues and update Excel export.
</commit_message>
<xml_diff>
--- a/Transformed_Spielplan_ExcelFormat.xlsx
+++ b/Transformed_Spielplan_ExcelFormat.xlsx
@@ -86,7 +86,7 @@
     <t/>
   </si>
   <si>
-    <t>Spieltag 8 - Th�ringenliga Damen | Spiel-ID: 1046 | Schiedsrichter: SV 1860 Oberwei�bach</t>
+    <t>Spieltag 8 - Thüringenliga Damen | Spiel-ID: 1046 | Schiedsrichter: SV 1860 Oberweißbach</t>
   </si>
   <si>
     <t>2025/26</t>
@@ -98,10 +98,10 @@
     <t>-</t>
   </si>
   <si>
-    <t>SV 1860 Oberwei�bach</t>
-  </si>
-  <si>
-    <t>Spieltag 8 - Th�ringenliga Damen | Spiel-ID: 1047 | Schiedsrichter: Geraer VC I</t>
+    <t>SV 1860 Oberweißbach</t>
+  </si>
+  <si>
+    <t>Spieltag 8 - Thüringenliga Damen | Spiel-ID: 1047 | Schiedsrichter: Geraer VC I</t>
   </si>
   <si>
     <t>VV70 Meiningen I</t>
@@ -113,22 +113,22 @@
     <t>Multihalle Meiningen (98617 Meiningen)</t>
   </si>
   <si>
-    <t>Spieltag 1 - Th�ringenliga Damen | Spiel-ID: 1004 | Schiedsrichter: SV 1860 Oberwei�bach</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spieltag 2 - Th�ringenliga Damen | Spiel-ID: 1010 | Schiedsrichter: SG  ERFURT electronic II</t>
+    <t>Spieltag 1 - Thüringenliga Damen | Spiel-ID: 1004 | Schiedsrichter: SV 1860 Oberweißbach</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spieltag 2 - Thüringenliga Damen | Spiel-ID: 1010 | Schiedsrichter: SG  ERFURT electronic II</t>
   </si>
   <si>
     <t xml:space="preserve">SG  ERFURT electronic II</t>
   </si>
   <si>
-    <t>Spieltag 2 - Th�ringenliga Damen | Spiel-ID: 1011 | Schiedsrichter: SV 1860 Oberwei�bach</t>
+    <t>Spieltag 2 - Thüringenliga Damen | Spiel-ID: 1011 | Schiedsrichter: SV 1860 Oberweißbach</t>
   </si>
   <si>
     <t>Gera Ostschule (07546 Gera)</t>
   </si>
   <si>
-    <t>Spieltag 3 - Th�ringenliga Damen | Spiel-ID: 1015 | Schiedsrichter: VV70 Meiningen I</t>
+    <t>Spieltag 3 - Thüringenliga Damen | Spiel-ID: 1015 | Schiedsrichter: VV70 Meiningen I</t>
   </si>
   <si>
     <t>SWE Volley-Team III</t>
@@ -137,73 +137,73 @@
     <t>Pierre-de-Coubertin Gymnasium (99096 Erfurt)</t>
   </si>
   <si>
-    <t>Spieltag 4 - Th�ringenliga Damen | Spiel-ID: 1023 | Schiedsrichter: SV 1860 Oberwei�bach</t>
+    <t>Spieltag 4 - Thüringenliga Damen | Spiel-ID: 1023 | Schiedsrichter: SV 1860 Oberweißbach</t>
   </si>
   <si>
     <t>Volleyball Gemeinschaft Bleicherode 1</t>
   </si>
   <si>
-    <t>Spieltag 6 - Th�ringenliga Damen | Spiel-ID: 1030 | Schiedsrichter: VC Altenburg I</t>
+    <t>Spieltag 6 - Thüringenliga Damen | Spiel-ID: 1030 | Schiedsrichter: VC Altenburg I</t>
   </si>
   <si>
     <t>VC Altenburg I</t>
   </si>
   <si>
-    <t>Spieltag 6 - Th�ringenliga Damen | Spiel-ID: 1031 | Schiedsrichter: Volleyball Gemeinschaft Bleicherode 1</t>
+    <t>Spieltag 6 - Thüringenliga Damen | Spiel-ID: 1031 | Schiedsrichter: Volleyball Gemeinschaft Bleicherode 1</t>
   </si>
   <si>
     <t>SVV Weimar e.V. I</t>
   </si>
   <si>
-    <t>Sporthalle Nordstra�e (99427 Weimar)</t>
-  </si>
-  <si>
-    <t>Spieltag 7 - Th�ringenliga Damen | Spiel-ID: 1038 | Schiedsrichter: VfB 91 Suhl II</t>
+    <t>Sporthalle Nordstraße (99427 Weimar)</t>
+  </si>
+  <si>
+    <t>Spieltag 7 - Thüringenliga Damen | Spiel-ID: 1038 | Schiedsrichter: VfB 91 Suhl II</t>
   </si>
   <si>
     <t>Wenzelhalle (04600 Altenburg)</t>
   </si>
   <si>
-    <t>Spieltag 10 - Th�ringenliga Damen | Spiel-ID: 1054 | Schiedsrichter: VV70 Meiningen I</t>
+    <t>Spieltag 10 - Thüringenliga Damen | Spiel-ID: 1054 | Schiedsrichter: VV70 Meiningen I</t>
   </si>
   <si>
     <t>VfB 91 Suhl II</t>
   </si>
   <si>
-    <t>SH Reinhard-He� (98529 Suhl)</t>
-  </si>
-  <si>
-    <t>Spieltag 5 - Th�ringenliga Damen | Spiel-ID: 1025 | Schiedsrichter: VV70 Meiningen I</t>
-  </si>
-  <si>
-    <t>Volley Juniors Th�ringen I</t>
-  </si>
-  <si>
-    <t>Spieltag 19 - Th�ringenliga Damen | Spiel-ID: 1097 | Schiedsrichter: -</t>
-  </si>
-  <si>
-    <t>Spieltag 12 - Th�ringenliga Damen | Spiel-ID: 1066 | Schiedsrichter: VfB 91 Suhl II</t>
-  </si>
-  <si>
-    <t>Spieltag 12 - Th�ringenliga Damen | Spiel-ID: 1067 | Schiedsrichter: VV70 Meiningen I</t>
+    <t>SH Reinhard-Heß (98529 Suhl)</t>
+  </si>
+  <si>
+    <t>Spieltag 5 - Thüringenliga Damen | Spiel-ID: 1025 | Schiedsrichter: VV70 Meiningen I</t>
+  </si>
+  <si>
+    <t>Volley Juniors Thüringen I</t>
+  </si>
+  <si>
+    <t>Spieltag 19 - Thüringenliga Damen | Spiel-ID: 1097 | Schiedsrichter: -</t>
+  </si>
+  <si>
+    <t>Spieltag 12 - Thüringenliga Damen | Spiel-ID: 1066 | Schiedsrichter: VfB 91 Suhl II</t>
+  </si>
+  <si>
+    <t>Spieltag 12 - Thüringenliga Damen | Spiel-ID: 1067 | Schiedsrichter: VV70 Meiningen I</t>
   </si>
   <si>
     <t>Georgenberg-SH (95752 Bleicherode)</t>
   </si>
   <si>
-    <t>Spieltag 13 - Th�ringenliga Damen | Spiel-ID: 1077 | Schiedsrichter: Geraer VC I</t>
+    <t>Spieltag 13 - Thüringenliga Damen | Spiel-ID: 1077 | Schiedsrichter: Geraer VC I</t>
   </si>
   <si>
     <t>SH Walter-Gropius-Schule Erfurt (99092 Erfurt)</t>
   </si>
   <si>
-    <t>Spieltag 14 - Th�ringenliga Damen | Spiel-ID: 1078 | Schiedsrichter: VV70 Meiningen I</t>
-  </si>
-  <si>
-    <t>Spieltag 15 - Th�ringenliga Damen | Spiel-ID: 1086 | Schiedsrichter: SWE Volley-Team III</t>
-  </si>
-  <si>
-    <t>Spieltag 15 - Th�ringenliga Damen | Spiel-ID: 1087 | Schiedsrichter: SVV Weimar e.V. I</t>
+    <t>Spieltag 14 - Thüringenliga Damen | Spiel-ID: 1078 | Schiedsrichter: VV70 Meiningen I</t>
+  </si>
+  <si>
+    <t>Spieltag 15 - Thüringenliga Damen | Spiel-ID: 1086 | Schiedsrichter: SWE Volley-Team III</t>
+  </si>
+  <si>
+    <t>Spieltag 15 - Thüringenliga Damen | Spiel-ID: 1087 | Schiedsrichter: SVV Weimar e.V. I</t>
   </si>
 </sst>
 </file>
@@ -275,7 +275,7 @@
     <col min="8" max="8" width="12.562342643737793" customWidth="1"/>
     <col min="9" max="9" width="42.68008041381836" customWidth="1"/>
     <col min="10" max="10" width="20.432785034179688" customWidth="1"/>
-    <col min="11" max="11" width="93.62908935546875" customWidth="1"/>
+    <col min="11" max="11" width="93.67169189453125" customWidth="1"/>
     <col min="12" max="12" width="25.051923751831055" customWidth="1"/>
     <col min="13" max="13" width="21.5837345123291" customWidth="1"/>
     <col min="14" max="14" width="42.23430252075195" customWidth="1"/>

</xml_diff>